<commit_message>
Added monthly overview to contract report
- replaced repository call, to avoid second database call in ContractReportDataMapper
</commit_message>
<xml_diff>
--- a/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
+++ b/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
@@ -13,10 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="Gesamtübersicht" sheetId="2" r:id="rId1"/>
-    <sheet name="Flags" sheetId="3" r:id="rId2"/>
+    <sheet name="Monatsübersicht" sheetId="5" r:id="rId2"/>
+    <sheet name="Flags" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gesamtübersicht!$B$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Monatsübersicht!$B$3:$I$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Leistungsstand</t>
   </si>
@@ -616,9 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -764,6 +764,154 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I9"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13">
+        <f>SUMIF(I4:I5,"{name}",E4:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <f>SUMIF(I4:I5,"{name}",F4:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <f>SUMIF(I4:I5,"{name}",G4:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16">
+        <f>SUM(E4:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="16">
+        <f>SUM(F4:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <f>SUM(G4:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
#171 Added net/gross view and switch link to budget overview
</commit_message>
<xml_diff>
--- a/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
+++ b/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarisaltik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wirz\git\budgeteer\budgeteer-web-interface\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtübersicht" sheetId="2" r:id="rId1"/>
@@ -618,29 +618,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -669,7 +667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -698,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
@@ -711,7 +709,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
@@ -733,7 +731,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
@@ -768,29 +766,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -819,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -848,7 +844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
@@ -861,7 +857,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
@@ -883,7 +879,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
@@ -922,9 +918,9 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Contract templates and the management for different templates types are complete
</commit_message>
<xml_diff>
--- a/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
+++ b/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wirz\git\budgeteer\budgeteer-web-interface\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atanasov\eclipse-workspace\budgeteer\budgeteer-web-interface\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Leistungsstand</t>
   </si>
@@ -105,6 +105,45 @@
   </si>
   <si>
     <t>Summe {name}</t>
+  </si>
+  <si>
+    <t>Accounting period</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Until</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Contract ID</t>
+  </si>
+  <si>
+    <t>Budget spent</t>
+  </si>
+  <si>
+    <t>Budget left</t>
+  </si>
+  <si>
+    <t>Budget total</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Invoice recipient</t>
+  </si>
+  <si>
+    <t>Sum according to invoice recipient</t>
+  </si>
+  <si>
+    <t>Sum {name}</t>
+  </si>
+  <si>
+    <t>Total sum</t>
   </si>
 </sst>
 </file>
@@ -618,56 +657,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -696,9 +737,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -709,9 +750,9 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -731,9 +772,9 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -768,25 +809,25 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -815,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -844,7 +885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
@@ -857,7 +898,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
@@ -879,7 +920,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
@@ -918,9 +959,9 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Translated template spreadsheet table names
</commit_message>
<xml_diff>
--- a/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
+++ b/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
@@ -12,13 +12,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12180"/>
   </bookViews>
   <sheets>
-    <sheet name="Gesamtübersicht" sheetId="2" r:id="rId1"/>
-    <sheet name="Monatsübersicht" sheetId="5" r:id="rId2"/>
+    <sheet name="Complete Overview" sheetId="2" r:id="rId1"/>
+    <sheet name="Month Overview" sheetId="5" r:id="rId2"/>
     <sheet name="Flags" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gesamtübersicht!$B$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Monatsübersicht!$B$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Complete Overview'!$B$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Month Overview'!$B$3:$I$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -622,25 +622,25 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -669,7 +669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -698,7 +698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
@@ -711,7 +711,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
@@ -772,25 +772,25 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -819,7 +819,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -848,7 +848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
@@ -861,7 +861,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -883,7 +883,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
@@ -922,9 +922,9 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
applied the changes requested in the review
</commit_message>
<xml_diff>
--- a/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
+++ b/budgeteer-web-interface/src/main/resources/contract-report-template.xlsx
@@ -618,9 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>